<commit_message>
unary and boolean operations
</commit_message>
<xml_diff>
--- a/docs/ParsingTable.xlsx
+++ b/docs/ParsingTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\compiler assignment\compiler\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68012292-F9E7-4520-9DF1-AE6BE7A6C14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C74B6A-B51A-4506-9F03-9CA914C5B67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{0022C85E-498E-4BD0-8DB9-B81496F666D8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t>Term</t>
   </si>
@@ -417,7 +417,27 @@
     </r>
   </si>
   <si>
-    <t>Literal | Identifier | … | SubExpr | …. |  PadRandI</t>
+    <t>Unary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(Subtract | Not) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expr</t>
+    </r>
+  </si>
+  <si>
+    <t>Subtract | Not</t>
+  </si>
+  <si>
+    <t>Literal | Identifier | Unary | SubExpr | …. |  PadRandI</t>
   </si>
 </sst>
 </file>
@@ -1039,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0976D8-5448-4256-BFD7-80DDB9F555E6}">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1113,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C68" si="0">IF(B4&lt;&gt;"","::=","")</f>
+        <f t="shared" ref="C4:C70" si="0">IF(B4&lt;&gt;"","::=","")</f>
         <v/>
       </c>
       <c r="D4" s="2"/>
@@ -1334,24 +1354,24 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="1" t="str">
-        <f>F14 &amp; "|…| BracOpen |… | PadRandI"</f>
-        <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |…| BracOpen |… | PadRandI</v>
+      <c r="D20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1368,140 +1388,140 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>F20</f>
-        <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |…| BracOpen |… | PadRandI</v>
+        <f>F14 &amp;"|" &amp;F20&amp;" |BracOpen |… | PadRandI"</f>
+        <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f>F22</f>
+        <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="1" t="str">
+      <c r="F25" s="1" t="str">
         <f>D16 &amp; "| ε"</f>
         <v>Multiply | Divide | ….| ε</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="1" t="str">
-        <f>F22</f>
-        <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |…| BracOpen |… | PadRandI</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f>F24</f>
+        <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>41</v>
       </c>
-      <c r="C26" t="str">
+      <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="1" t="str">
+      <c r="F28" s="1" t="str">
         <f>D17 &amp;" | ε"</f>
         <v>Add | Subtract | ….  | ε</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="1" t="str">
-        <f>F25</f>
-        <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |…| BracOpen |… | PadRandI</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="1" t="str">
-        <f>D18&amp;" | ε"</f>
-        <v>LT | GT | EQ | NE | LTE | GTE | ε</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>::=</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <f>F27</f>
+        <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1509,17 +1529,18 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>54</v>
+      <c r="D31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <f>D18&amp;" | ε"</f>
+        <v>LT | GT | EQ | NE | LTE | GTE | ε</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1531,16 +1552,25 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>::=</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1549,7 +1579,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1558,7 +1588,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1567,7 +1597,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1576,7 +1606,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1585,7 +1615,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1594,7 +1624,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1603,7 +1633,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1612,7 +1642,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1621,7 +1651,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1630,7 +1660,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1639,7 +1669,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1648,7 +1678,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1657,7 +1687,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1666,7 +1696,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1860,7 +1890,7 @@
         <v>67</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" ref="C69:C74" si="1">IF(B69&lt;&gt;"","::=","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1869,7 +1899,7 @@
         <v>68</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1878,7 +1908,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C71:C76" si="1">IF(B71&lt;&gt;"","::=","")</f>
         <v/>
       </c>
     </row>
@@ -1913,11 +1943,19 @@
       <c r="A75">
         <v>73</v>
       </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
@@ -2232,6 +2270,16 @@
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
padrandi padread and actualparams
</commit_message>
<xml_diff>
--- a/docs/ParsingTable.xlsx
+++ b/docs/ParsingTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wayne\Desktop\cps2000 compiler\CPS2000-compiler\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\compiler assignment\compiler\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375EF36F-084D-4901-B661-7C74897FA309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4B12E3-5F8E-4913-8D34-B5F864F3A797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0022C85E-498E-4BD0-8DB9-B81496F666D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{0022C85E-498E-4BD0-8DB9-B81496F666D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -914,23 +914,23 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
@@ -971,7 +971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -997,7 +997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1061,32 +1061,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
         <v>3</v>
       </c>
@@ -1119,19 +1119,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0976D8-5448-4256-BFD7-80DDB9F555E6}">
   <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>Multiply | Divide | ….| ε</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>Add | Subtract | ….  | ε</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>LT | GT | EQ | NE | LTE | GTE | ε</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>True | False | Int | Float | Colour | PadWidth | PadHeight | PadRead | PadRandI |Subtract | Not |BracOpen |… | PadRandI</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -2034,327 +2034,327 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>

</xml_diff>